<commit_message>
Plots of KPI's + moved old files
</commit_message>
<xml_diff>
--- a/Data/Results statistical moments.xlsx
+++ b/Data/Results statistical moments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fiasa\Documents\KUL\Thesis\Code\Thesis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB03B624-7BA1-4681-B7B0-76687DCE28EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9668FB9-1EB6-47BD-AE06-493801CD6C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{5A4657A2-0C5A-47DB-9C73-D80A6BC4E9EC}"/>
   </bookViews>
@@ -504,6 +504,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -511,9 +514,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -855,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF4CA1A-BCD5-499B-A6AC-3DDC80109A15}">
   <dimension ref="B1:BS41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" zoomScale="91" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="S34" sqref="S34"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -911,11 +911,11 @@
   <sheetData>
     <row r="1" spans="2:71" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:71" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="27"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="28"/>
       <c r="H2" s="3" t="s">
         <v>1</v>
       </c>
@@ -937,101 +937,101 @@
       <c r="N2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="28" t="s">
+      <c r="O2" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="27"/>
       <c r="R2" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="S2" s="25"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="25" t="s">
+      <c r="S2" s="26"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="25"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="28" t="s">
+      <c r="V2" s="26"/>
+      <c r="W2" s="28"/>
+      <c r="X2" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="Y2" s="25"/>
-      <c r="Z2" s="26"/>
-      <c r="AA2" s="25" t="s">
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="AB2" s="25"/>
-      <c r="AC2" s="25"/>
-      <c r="AD2" s="25" t="s">
+      <c r="AB2" s="26"/>
+      <c r="AC2" s="26"/>
+      <c r="AD2" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="AE2" s="25"/>
-      <c r="AF2" s="26"/>
-      <c r="AG2" s="25" t="s">
+      <c r="AE2" s="26"/>
+      <c r="AF2" s="27"/>
+      <c r="AG2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="AH2" s="25"/>
-      <c r="AI2" s="27"/>
-      <c r="AJ2" s="28" t="s">
+      <c r="AH2" s="26"/>
+      <c r="AI2" s="28"/>
+      <c r="AJ2" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="26"/>
+      <c r="AK2" s="26"/>
+      <c r="AL2" s="27"/>
       <c r="AM2" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="AN2" s="25"/>
-      <c r="AO2" s="26"/>
+      <c r="AN2" s="26"/>
+      <c r="AO2" s="27"/>
       <c r="AP2" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="AQ2" s="25"/>
-      <c r="AR2" s="26"/>
+      <c r="AQ2" s="26"/>
+      <c r="AR2" s="27"/>
       <c r="AS2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="AT2" s="25"/>
-      <c r="AU2" s="26"/>
+      <c r="AT2" s="26"/>
+      <c r="AU2" s="27"/>
       <c r="AV2" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="AW2" s="25"/>
-      <c r="AX2" s="26"/>
+      <c r="AW2" s="26"/>
+      <c r="AX2" s="27"/>
       <c r="AY2" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="AZ2" s="25"/>
-      <c r="BA2" s="26"/>
+      <c r="AZ2" s="26"/>
+      <c r="BA2" s="27"/>
       <c r="BB2" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="BC2" s="25"/>
-      <c r="BD2" s="26"/>
+      <c r="BC2" s="26"/>
+      <c r="BD2" s="27"/>
       <c r="BE2" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="BF2" s="25"/>
-      <c r="BG2" s="26"/>
+      <c r="BF2" s="26"/>
+      <c r="BG2" s="27"/>
       <c r="BH2" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="BI2" s="25"/>
-      <c r="BJ2" s="26"/>
+      <c r="BI2" s="26"/>
+      <c r="BJ2" s="27"/>
       <c r="BK2" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="BL2" s="25"/>
-      <c r="BM2" s="26"/>
+      <c r="BL2" s="26"/>
+      <c r="BM2" s="27"/>
       <c r="BN2" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="BO2" s="25"/>
-      <c r="BP2" s="26"/>
-      <c r="BQ2" s="25" t="s">
+      <c r="BO2" s="26"/>
+      <c r="BP2" s="27"/>
+      <c r="BQ2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="BR2" s="25"/>
-      <c r="BS2" s="27"/>
+      <c r="BR2" s="26"/>
+      <c r="BS2" s="28"/>
     </row>
     <row r="3" spans="2:71" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D3" t="s">
@@ -1695,7 +1695,7 @@
         <v>0.63</v>
       </c>
       <c r="R6" s="16">
-        <v>-0.06</v>
+        <v>-0.6</v>
       </c>
       <c r="S6">
         <v>-0.38</v>
@@ -2072,11 +2072,11 @@
       <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="27"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="28"/>
       <c r="H10" s="3" t="s">
         <v>1</v>
       </c>
@@ -2098,101 +2098,101 @@
       <c r="N10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="O10" s="28" t="s">
+      <c r="O10" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="25" t="s">
+      <c r="P10" s="26"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="S10" s="25"/>
-      <c r="T10" s="26"/>
-      <c r="U10" s="25" t="s">
+      <c r="S10" s="26"/>
+      <c r="T10" s="27"/>
+      <c r="U10" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="V10" s="25"/>
-      <c r="W10" s="27"/>
-      <c r="X10" s="28" t="s">
+      <c r="V10" s="26"/>
+      <c r="W10" s="28"/>
+      <c r="X10" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="Y10" s="25"/>
-      <c r="Z10" s="26"/>
-      <c r="AA10" s="25" t="s">
+      <c r="Y10" s="26"/>
+      <c r="Z10" s="27"/>
+      <c r="AA10" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="AB10" s="25"/>
-      <c r="AC10" s="26"/>
-      <c r="AD10" s="25" t="s">
+      <c r="AB10" s="26"/>
+      <c r="AC10" s="27"/>
+      <c r="AD10" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="AE10" s="25"/>
-      <c r="AF10" s="26"/>
-      <c r="AG10" s="25" t="s">
+      <c r="AE10" s="26"/>
+      <c r="AF10" s="27"/>
+      <c r="AG10" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="AH10" s="25"/>
-      <c r="AI10" s="27"/>
-      <c r="AJ10" s="28" t="s">
+      <c r="AH10" s="26"/>
+      <c r="AI10" s="28"/>
+      <c r="AJ10" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="AK10" s="25"/>
-      <c r="AL10" s="26"/>
-      <c r="AM10" s="25" t="s">
+      <c r="AK10" s="26"/>
+      <c r="AL10" s="27"/>
+      <c r="AM10" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="AN10" s="25"/>
-      <c r="AO10" s="26"/>
-      <c r="AP10" s="25" t="s">
+      <c r="AN10" s="26"/>
+      <c r="AO10" s="27"/>
+      <c r="AP10" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AQ10" s="25"/>
-      <c r="AR10" s="26"/>
-      <c r="AS10" s="25" t="s">
+      <c r="AQ10" s="26"/>
+      <c r="AR10" s="27"/>
+      <c r="AS10" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="AT10" s="25"/>
-      <c r="AU10" s="26"/>
-      <c r="AV10" s="25" t="s">
+      <c r="AT10" s="26"/>
+      <c r="AU10" s="27"/>
+      <c r="AV10" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="AW10" s="25"/>
-      <c r="AX10" s="26"/>
-      <c r="AY10" s="25" t="s">
+      <c r="AW10" s="26"/>
+      <c r="AX10" s="27"/>
+      <c r="AY10" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="AZ10" s="25"/>
-      <c r="BA10" s="26"/>
-      <c r="BB10" s="25" t="s">
+      <c r="AZ10" s="26"/>
+      <c r="BA10" s="27"/>
+      <c r="BB10" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="BC10" s="25"/>
-      <c r="BD10" s="26"/>
-      <c r="BE10" s="25" t="s">
+      <c r="BC10" s="26"/>
+      <c r="BD10" s="27"/>
+      <c r="BE10" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="BF10" s="25"/>
-      <c r="BG10" s="26"/>
-      <c r="BH10" s="25" t="s">
+      <c r="BF10" s="26"/>
+      <c r="BG10" s="27"/>
+      <c r="BH10" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="BI10" s="25"/>
-      <c r="BJ10" s="26"/>
-      <c r="BK10" s="25" t="s">
+      <c r="BI10" s="26"/>
+      <c r="BJ10" s="27"/>
+      <c r="BK10" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="BL10" s="25"/>
-      <c r="BM10" s="26"/>
-      <c r="BN10" s="25" t="s">
+      <c r="BL10" s="26"/>
+      <c r="BM10" s="27"/>
+      <c r="BN10" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="BO10" s="25"/>
-      <c r="BP10" s="26"/>
-      <c r="BQ10" s="25" t="s">
+      <c r="BO10" s="26"/>
+      <c r="BP10" s="27"/>
+      <c r="BQ10" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="BR10" s="25"/>
-      <c r="BS10" s="27"/>
+      <c r="BR10" s="26"/>
+      <c r="BS10" s="28"/>
     </row>
     <row r="11" spans="2:71" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" t="s">
@@ -2436,7 +2436,7 @@
         <v>0.63</v>
       </c>
       <c r="R12" s="5">
-        <v>-0.06</v>
+        <v>-0.6</v>
       </c>
       <c r="S12" s="5">
         <v>-0.38</v>
@@ -4915,11 +4915,11 @@
       <c r="B28" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="28" t="s">
+      <c r="E28" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="F28" s="25"/>
-      <c r="G28" s="27"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="28"/>
       <c r="H28" s="3" t="s">
         <v>1</v>
       </c>
@@ -4941,101 +4941,101 @@
       <c r="N28" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="O28" s="28" t="s">
+      <c r="O28" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="P28" s="25"/>
-      <c r="Q28" s="26"/>
-      <c r="R28" s="25" t="s">
+      <c r="P28" s="26"/>
+      <c r="Q28" s="27"/>
+      <c r="R28" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="S28" s="25"/>
-      <c r="T28" s="26"/>
-      <c r="U28" s="25" t="s">
+      <c r="S28" s="26"/>
+      <c r="T28" s="27"/>
+      <c r="U28" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="V28" s="25"/>
-      <c r="W28" s="27"/>
-      <c r="X28" s="28" t="s">
+      <c r="V28" s="26"/>
+      <c r="W28" s="28"/>
+      <c r="X28" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="Y28" s="25"/>
-      <c r="Z28" s="26"/>
-      <c r="AA28" s="25" t="s">
+      <c r="Y28" s="26"/>
+      <c r="Z28" s="27"/>
+      <c r="AA28" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="AB28" s="25"/>
-      <c r="AC28" s="26"/>
-      <c r="AD28" s="25" t="s">
+      <c r="AB28" s="26"/>
+      <c r="AC28" s="27"/>
+      <c r="AD28" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="AE28" s="25"/>
-      <c r="AF28" s="26"/>
-      <c r="AG28" s="25" t="s">
+      <c r="AE28" s="26"/>
+      <c r="AF28" s="27"/>
+      <c r="AG28" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="AH28" s="25"/>
-      <c r="AI28" s="27"/>
-      <c r="AJ28" s="28" t="s">
+      <c r="AH28" s="26"/>
+      <c r="AI28" s="28"/>
+      <c r="AJ28" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="AK28" s="25"/>
-      <c r="AL28" s="26"/>
-      <c r="AM28" s="25" t="s">
+      <c r="AK28" s="26"/>
+      <c r="AL28" s="27"/>
+      <c r="AM28" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="AN28" s="25"/>
-      <c r="AO28" s="26"/>
-      <c r="AP28" s="25" t="s">
+      <c r="AN28" s="26"/>
+      <c r="AO28" s="27"/>
+      <c r="AP28" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AQ28" s="25"/>
-      <c r="AR28" s="26"/>
-      <c r="AS28" s="25" t="s">
+      <c r="AQ28" s="26"/>
+      <c r="AR28" s="27"/>
+      <c r="AS28" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="AT28" s="25"/>
-      <c r="AU28" s="26"/>
-      <c r="AV28" s="25" t="s">
+      <c r="AT28" s="26"/>
+      <c r="AU28" s="27"/>
+      <c r="AV28" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="AW28" s="25"/>
-      <c r="AX28" s="26"/>
-      <c r="AY28" s="25" t="s">
+      <c r="AW28" s="26"/>
+      <c r="AX28" s="27"/>
+      <c r="AY28" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="AZ28" s="25"/>
-      <c r="BA28" s="26"/>
-      <c r="BB28" s="25" t="s">
+      <c r="AZ28" s="26"/>
+      <c r="BA28" s="27"/>
+      <c r="BB28" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="BC28" s="25"/>
-      <c r="BD28" s="26"/>
-      <c r="BE28" s="25" t="s">
+      <c r="BC28" s="26"/>
+      <c r="BD28" s="27"/>
+      <c r="BE28" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="BF28" s="25"/>
-      <c r="BG28" s="26"/>
-      <c r="BH28" s="25" t="s">
+      <c r="BF28" s="26"/>
+      <c r="BG28" s="27"/>
+      <c r="BH28" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="BI28" s="25"/>
-      <c r="BJ28" s="26"/>
-      <c r="BK28" s="25" t="s">
+      <c r="BI28" s="26"/>
+      <c r="BJ28" s="27"/>
+      <c r="BK28" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="BL28" s="25"/>
-      <c r="BM28" s="26"/>
-      <c r="BN28" s="25" t="s">
+      <c r="BL28" s="26"/>
+      <c r="BM28" s="27"/>
+      <c r="BN28" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="BO28" s="25"/>
-      <c r="BP28" s="26"/>
-      <c r="BQ28" s="25" t="s">
+      <c r="BO28" s="26"/>
+      <c r="BP28" s="27"/>
+      <c r="BQ28" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="BR28" s="25"/>
-      <c r="BS28" s="27"/>
+      <c r="BR28" s="26"/>
+      <c r="BS28" s="28"/>
     </row>
     <row r="29" spans="2:71" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C29" t="s">
@@ -7755,38 +7755,18 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="X10:Z10"/>
-    <mergeCell ref="AA10:AC10"/>
-    <mergeCell ref="AD10:AF10"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="U10:W10"/>
-    <mergeCell ref="BN10:BP10"/>
-    <mergeCell ref="BQ10:BS10"/>
-    <mergeCell ref="AJ10:AL10"/>
-    <mergeCell ref="AM10:AO10"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="AS10:AU10"/>
-    <mergeCell ref="AV10:AX10"/>
-    <mergeCell ref="AY10:BA10"/>
-    <mergeCell ref="AA2:AC2"/>
-    <mergeCell ref="BB10:BD10"/>
-    <mergeCell ref="BE10:BG10"/>
-    <mergeCell ref="BH10:BJ10"/>
-    <mergeCell ref="BK10:BM10"/>
-    <mergeCell ref="AG10:AI10"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="U2:W2"/>
-    <mergeCell ref="X2:Z2"/>
-    <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="AJ2:AL2"/>
-    <mergeCell ref="AM2:AO2"/>
-    <mergeCell ref="AP2:AR2"/>
-    <mergeCell ref="AS2:AU2"/>
+    <mergeCell ref="BQ28:BS28"/>
+    <mergeCell ref="AJ28:AL28"/>
+    <mergeCell ref="AM28:AO28"/>
+    <mergeCell ref="AP28:AR28"/>
+    <mergeCell ref="AS28:AU28"/>
+    <mergeCell ref="AV28:AX28"/>
+    <mergeCell ref="AY28:BA28"/>
+    <mergeCell ref="BB28:BD28"/>
+    <mergeCell ref="BE28:BG28"/>
+    <mergeCell ref="BH28:BJ28"/>
+    <mergeCell ref="BK28:BM28"/>
+    <mergeCell ref="BN28:BP28"/>
     <mergeCell ref="BN2:BP2"/>
     <mergeCell ref="BQ2:BS2"/>
     <mergeCell ref="O28:Q28"/>
@@ -7803,18 +7783,38 @@
     <mergeCell ref="BH2:BJ2"/>
     <mergeCell ref="BK2:BM2"/>
     <mergeCell ref="AD2:AF2"/>
-    <mergeCell ref="BQ28:BS28"/>
-    <mergeCell ref="AJ28:AL28"/>
-    <mergeCell ref="AM28:AO28"/>
-    <mergeCell ref="AP28:AR28"/>
-    <mergeCell ref="AS28:AU28"/>
-    <mergeCell ref="AV28:AX28"/>
-    <mergeCell ref="AY28:BA28"/>
-    <mergeCell ref="BB28:BD28"/>
-    <mergeCell ref="BE28:BG28"/>
-    <mergeCell ref="BH28:BJ28"/>
-    <mergeCell ref="BK28:BM28"/>
-    <mergeCell ref="BN28:BP28"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="U2:W2"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="AA2:AC2"/>
+    <mergeCell ref="BB10:BD10"/>
+    <mergeCell ref="BE10:BG10"/>
+    <mergeCell ref="BH10:BJ10"/>
+    <mergeCell ref="BK10:BM10"/>
+    <mergeCell ref="AG10:AI10"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="AJ2:AL2"/>
+    <mergeCell ref="AM2:AO2"/>
+    <mergeCell ref="AP2:AR2"/>
+    <mergeCell ref="AS2:AU2"/>
+    <mergeCell ref="BN10:BP10"/>
+    <mergeCell ref="BQ10:BS10"/>
+    <mergeCell ref="AJ10:AL10"/>
+    <mergeCell ref="AM10:AO10"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="AS10:AU10"/>
+    <mergeCell ref="AV10:AX10"/>
+    <mergeCell ref="AY10:BA10"/>
+    <mergeCell ref="X10:Z10"/>
+    <mergeCell ref="AA10:AC10"/>
+    <mergeCell ref="AD10:AF10"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="U10:W10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>